<commit_message>
fixed trv and file name
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateRDT.xlsx
+++ b/TeplosilaWeb/Content/templates/templateRDT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{F7AA5767-6F95-4FDE-BBF4-12E955C09F42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E8B6FBA5-8BEA-47AF-AD7B-F3D739782D94}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{F7AA5767-6F95-4FDE-BBF4-12E955C09F42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8B0E4620-6FCC-4F0E-8B8F-566371C03277}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -573,7 +573,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -581,8 +581,8 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>10835</xdr:rowOff>
     </xdr:to>
@@ -596,7 +596,7 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -614,7 +614,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1"/>
-          <a:ext cx="6635750" cy="804584"/>
+          <a:ext cx="6326188" cy="804584"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -892,7 +892,7 @@
   <dimension ref="A1:W81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
redesign trv and rdt
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateRDT.xlsx
+++ b/TeplosilaWeb/Content/templates/templateRDT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22451d98f477d1d3/Рабочий стол/TeploSilaWeb/TeplosilaWeb/Content/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\Рабочая папка\ТЗ программа подбора TRV, RDT\templates\Новые RDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{F7AA5767-6F95-4FDE-BBF4-12E955C09F42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8B0E4620-6FCC-4F0E-8B8F-566371C03277}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="11265"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Номинальный диаметр DN, мм</t>
   </si>
@@ -68,9 +67,6 @@
     <t>Объект:</t>
   </si>
   <si>
-    <t>Место установки:</t>
-  </si>
-  <si>
     <t>Входные данные</t>
   </si>
   <si>
@@ -126,18 +122,12 @@
     <t>Исполнение регулятора:</t>
   </si>
   <si>
-    <t>Регулятор давления "после себя"</t>
-  </si>
-  <si>
     <t>Марка регулятора:</t>
   </si>
   <si>
     <t>Потери давления на клапане регулятора:</t>
   </si>
   <si>
-    <t>Регулятор перепада давления</t>
-  </si>
-  <si>
     <t>Потери давления на регуляторе   ΔPрд=</t>
   </si>
   <si>
@@ -148,24 +138,6 @@
   </si>
   <si>
     <t>бар</t>
-  </si>
-  <si>
-    <t>Требуемое давление после регулятора   Р(треб)=</t>
-  </si>
-  <si>
-    <t>Давление перед регулятором   Р'1=</t>
-  </si>
-  <si>
-    <t>Регулятор давления "до себя"</t>
-  </si>
-  <si>
-    <t>Требуемое давление перед регулятором   Р(треб)=</t>
-  </si>
-  <si>
-    <t>Давление после регулятора   Р'2=</t>
-  </si>
-  <si>
-    <t>Регулятор "перепуска"</t>
   </si>
   <si>
     <t>Расчет регулятора давления на кавитацию:</t>
@@ -216,11 +188,6 @@
     <t>Масса m=</t>
   </si>
   <si>
-    <t>В комплекте с регуляторами давления поставляются импульсные трубки в количестве:
-- с регуляторами перепада давления RDT и регуляторами "перепуска" RDT-B - 2 шт.;
-- с регуляторами давления "после себя" RDT-P и регуляторами давления "до себя" RDT-S - 1 шт.</t>
-  </si>
-  <si>
     <t>Марка регулятора давления</t>
   </si>
   <si>
@@ -237,12 +204,18 @@
   </si>
   <si>
     <t>Пропускная способность Kvs, м³/ч</t>
+  </si>
+  <si>
+    <t>В комплекте с регуляторами перепада давления RDT поставляются:
+- медная импульсная трубка - 2 шт.;
+- латунная гайка - 4 шт.;
+- латунный штуцер - 2 шт.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,9 +404,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -467,6 +437,57 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -485,74 +506,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,11 +843,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="A31" sqref="A31:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,12 +874,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="38"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -939,19 +894,19 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -966,19 +921,19 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="42"/>
+      <c r="A4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -993,19 +948,19 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="42"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1019,20 +974,18 @@
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="45"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1046,18 +999,20 @@
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1072,19 +1027,19 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -1098,11 +1053,11 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="34"/>
+    <row r="9" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -1125,20 +1080,20 @@
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
+    <row r="10" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1153,19 +1108,19 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="A11" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1181,7 +1136,7 @@
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
@@ -1190,9 +1145,9 @@
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="16"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1208,7 +1163,7 @@
     </row>
     <row r="13" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
@@ -1217,9 +1172,9 @@
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="16"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1235,7 +1190,7 @@
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
@@ -1244,9 +1199,11 @@
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="16"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1260,36 +1217,36 @@
       <c r="V14" s="2"/>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="16"/>
+    <row r="15" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
@@ -1298,135 +1255,139 @@
       <c r="F16" s="27"/>
       <c r="G16" s="27"/>
       <c r="H16" s="27"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="16" t="s">
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+    </row>
+    <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+    </row>
+    <row r="18" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+    </row>
+    <row r="19" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-    </row>
-    <row r="18" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-    </row>
-    <row r="19" spans="1:23" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+    </row>
+    <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-    </row>
-    <row r="20" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
     </row>
     <row r="21" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -1435,25 +1396,25 @@
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="16"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="15"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
     </row>
     <row r="22" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
@@ -1462,9 +1423,9 @@
       <c r="F22" s="27"/>
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="16"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="15"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -1478,269 +1439,271 @@
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
+    <row r="23" spans="1:23" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="4"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="16"/>
+      <c r="A24" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-    </row>
-    <row r="25" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="16"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-    </row>
-    <row r="27" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="16" t="s">
-        <v>11</v>
-      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23" s="1" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-    </row>
-    <row r="28" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" spans="1:23" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="39"/>
+      <c r="F28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="L28" s="2"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-      <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-    </row>
-    <row r="29" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="16" t="s">
-        <v>11</v>
-      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="1:23" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="9"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-    </row>
-    <row r="30" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="16" t="s">
-        <v>11</v>
-      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-    </row>
-    <row r="31" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="16"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" s="1" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-    </row>
-    <row r="32" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="16"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -1754,18 +1717,21 @@
       <c r="V32" s="2"/>
       <c r="W32" s="2"/>
     </row>
-    <row r="33" spans="1:23" s="1" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="4"/>
+    <row r="33" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="D33" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="34"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -1779,16 +1745,17 @@
       <c r="V33" s="2"/>
       <c r="W33" s="2"/>
     </row>
-    <row r="34" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+    <row r="34" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="D34" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="34"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -1806,20 +1773,21 @@
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
     </row>
-    <row r="35" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
+    <row r="35" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="D35" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="34"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -1833,20 +1801,21 @@
       <c r="V35" s="2"/>
       <c r="W35" s="2"/>
     </row>
-    <row r="36" spans="1:23" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
+    <row r="36" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="D36" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="36"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -1860,11 +1829,11 @@
       <c r="V36" s="2"/>
       <c r="W36" s="2"/>
     </row>
-    <row r="37" spans="1:23" s="1" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+    <row r="37" spans="1:23" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -1885,37 +1854,15 @@
       <c r="V37" s="2"/>
       <c r="W37" s="2"/>
     </row>
-    <row r="38" spans="1:23" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I38" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="J38" s="26"/>
-      <c r="K38" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="L38" s="2"/>
+    <row r="38" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -1928,19 +1875,15 @@
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
     </row>
-    <row r="39" spans="1:23" s="1" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="2"/>
+    <row r="39" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -1953,21 +1896,15 @@
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
     </row>
-    <row r="40" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="2"/>
+    <row r="40" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -1980,21 +1917,15 @@
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
     </row>
-    <row r="41" spans="1:23" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="2"/>
+    <row r="41" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -2010,11 +1941,11 @@
     <row r="42" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="6"/>
+      <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
@@ -2035,14 +1966,11 @@
     <row r="43" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="D43" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -2063,14 +1991,11 @@
     <row r="44" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
-      <c r="D44" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
@@ -2091,14 +2016,11 @@
     <row r="45" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="D45" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
@@ -2119,14 +2041,11 @@
     <row r="46" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="D46" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
@@ -2144,11 +2063,11 @@
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
     </row>
-    <row r="47" spans="1:23" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -2178,6 +2097,10 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -2199,6 +2122,10 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -2211,7 +2138,7 @@
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
     </row>
-    <row r="50" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2220,6 +2147,10 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -2241,6 +2172,10 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -2528,7 +2463,7 @@
       <c r="V62" s="2"/>
       <c r="W62" s="2"/>
     </row>
-    <row r="63" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2553,7 +2488,7 @@
       <c r="V63" s="2"/>
       <c r="W63" s="2"/>
     </row>
-    <row r="64" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2578,7 +2513,7 @@
       <c r="V64" s="2"/>
       <c r="W64" s="2"/>
     </row>
-    <row r="65" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2603,7 +2538,7 @@
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
     </row>
-    <row r="66" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2628,7 +2563,7 @@
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
     </row>
-    <row r="67" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2653,7 +2588,7 @@
       <c r="V67" s="2"/>
       <c r="W67" s="2"/>
     </row>
-    <row r="68" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2678,7 +2613,7 @@
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
     </row>
-    <row r="69" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2703,7 +2638,7 @@
       <c r="V69" s="2"/>
       <c r="W69" s="2"/>
     </row>
-    <row r="70" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2728,7 +2663,7 @@
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
     </row>
-    <row r="71" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2753,325 +2688,59 @@
       <c r="V71" s="2"/>
       <c r="W71" s="2"/>
     </row>
-    <row r="72" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="2"/>
-      <c r="M72" s="2"/>
-      <c r="N72" s="2"/>
-      <c r="O72" s="2"/>
-      <c r="P72" s="2"/>
-      <c r="Q72" s="2"/>
-      <c r="R72" s="2"/>
-      <c r="S72" s="2"/>
-      <c r="T72" s="2"/>
-      <c r="U72" s="2"/>
-      <c r="V72" s="2"/>
-      <c r="W72" s="2"/>
-    </row>
-    <row r="73" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
-      <c r="O73" s="2"/>
-      <c r="P73" s="2"/>
-      <c r="Q73" s="2"/>
-      <c r="R73" s="2"/>
-      <c r="S73" s="2"/>
-      <c r="T73" s="2"/>
-      <c r="U73" s="2"/>
-      <c r="V73" s="2"/>
-      <c r="W73" s="2"/>
-    </row>
-    <row r="74" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="2"/>
-      <c r="M74" s="2"/>
-      <c r="N74" s="2"/>
-      <c r="O74" s="2"/>
-      <c r="P74" s="2"/>
-      <c r="Q74" s="2"/>
-      <c r="R74" s="2"/>
-      <c r="S74" s="2"/>
-      <c r="T74" s="2"/>
-      <c r="U74" s="2"/>
-      <c r="V74" s="2"/>
-      <c r="W74" s="2"/>
-    </row>
-    <row r="75" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="2"/>
-      <c r="M75" s="2"/>
-      <c r="N75" s="2"/>
-      <c r="O75" s="2"/>
-      <c r="P75" s="2"/>
-      <c r="Q75" s="2"/>
-      <c r="R75" s="2"/>
-      <c r="S75" s="2"/>
-      <c r="T75" s="2"/>
-      <c r="U75" s="2"/>
-      <c r="V75" s="2"/>
-      <c r="W75" s="2"/>
-    </row>
-    <row r="76" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
-      <c r="Q76" s="2"/>
-      <c r="R76" s="2"/>
-      <c r="S76" s="2"/>
-      <c r="T76" s="2"/>
-      <c r="U76" s="2"/>
-      <c r="V76" s="2"/>
-      <c r="W76" s="2"/>
-    </row>
-    <row r="77" spans="1:23" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="2"/>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
-      <c r="R77" s="2"/>
-      <c r="S77" s="2"/>
-      <c r="T77" s="2"/>
-      <c r="U77" s="2"/>
-      <c r="V77" s="2"/>
-      <c r="W77" s="2"/>
-    </row>
-    <row r="78" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="2"/>
-      <c r="S78" s="2"/>
-      <c r="T78" s="2"/>
-      <c r="U78" s="2"/>
-      <c r="V78" s="2"/>
-      <c r="W78" s="2"/>
-    </row>
-    <row r="79" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
-      <c r="Q79" s="2"/>
-      <c r="R79" s="2"/>
-      <c r="S79" s="2"/>
-      <c r="T79" s="2"/>
-      <c r="U79" s="2"/>
-      <c r="V79" s="2"/>
-      <c r="W79" s="2"/>
-    </row>
-    <row r="80" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
-      <c r="O80" s="2"/>
-      <c r="P80" s="2"/>
-      <c r="Q80" s="2"/>
-      <c r="R80" s="2"/>
-      <c r="S80" s="2"/>
-      <c r="T80" s="2"/>
-      <c r="U80" s="2"/>
-      <c r="V80" s="2"/>
-      <c r="W80" s="2"/>
-    </row>
-    <row r="81" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-      <c r="L81" s="2"/>
-      <c r="M81" s="2"/>
-      <c r="N81" s="2"/>
-      <c r="O81" s="2"/>
-      <c r="P81" s="2"/>
-      <c r="Q81" s="2"/>
-      <c r="R81" s="2"/>
-      <c r="S81" s="2"/>
-      <c r="T81" s="2"/>
-      <c r="U81" s="2"/>
-      <c r="V81" s="2"/>
-      <c r="W81" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="51">
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A18:K18"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="E26:K26"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:K8"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:K25"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:K4"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:K5"/>
-    <mergeCell ref="C6:K6"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="E36:K36"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="E35:K35"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:K20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A28:K28"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A32:H32"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>